<commit_message>
FIX: some fixes to the lexical scanner FSM.
</commit_message>
<xml_diff>
--- a/docs/lexer-FSM.xlsx
+++ b/docs/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26903664-7424-47E4-A237-C534825D9C6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="20" windowWidth="21060" windowHeight="18580" tabRatio="564"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transitions" sheetId="2" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="93">
   <si>
     <t>S_START</t>
   </si>
@@ -288,12 +294,18 @@
   </si>
   <si>
     <t>T_ISSUE</t>
+  </si>
+  <si>
+    <t>T_INTEGER</t>
+  </si>
+  <si>
+    <t>T_PERCENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -334,12 +346,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -383,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -402,6 +420,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,6 +432,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -459,7 +483,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,9 +516,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -527,6 +568,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -702,30 +760,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S36" sqref="S36"/>
+      <selection pane="topRight" activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="6" width="8.08984375" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.08984375" customWidth="1"/>
-    <col min="13" max="13" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.08984375" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" customWidth="1"/>
+    <col min="2" max="6" width="8.06640625" customWidth="1"/>
+    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.06640625" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.06640625" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.08984375" customWidth="1"/>
-    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="42" width="8.08984375" customWidth="1"/>
+    <col min="16" max="17" width="8.06640625" customWidth="1"/>
+    <col min="18" max="18" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="19" max="42" width="8.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -851,7 +909,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>39</v>
       </c>
@@ -909,7 +967,9 @@
       <c r="S2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T2" s="6"/>
+      <c r="T2" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
@@ -933,7 +993,7 @@
       <c r="AO2" s="6"/>
       <c r="AP2" s="6"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -991,7 +1051,9 @@
       <c r="S3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T3" s="6"/>
+      <c r="T3" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
@@ -1015,11 +1077,13 @@
       <c r="AO3" s="6"/>
       <c r="AP3" s="6"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1135,9 @@
       <c r="S4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T4" s="6"/>
+      <c r="T4" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
@@ -1095,11 +1161,13 @@
       <c r="AO4" s="6"/>
       <c r="AP4" s="6"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1219,9 @@
       <c r="S5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T5" s="6"/>
+      <c r="T5" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
@@ -1175,7 +1245,7 @@
       <c r="AO5" s="6"/>
       <c r="AP5" s="6"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -1233,7 +1303,9 @@
       <c r="S6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T6" s="6"/>
+      <c r="T6" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
@@ -1257,7 +1329,7 @@
       <c r="AO6" s="6"/>
       <c r="AP6" s="6"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>44</v>
       </c>
@@ -1315,7 +1387,9 @@
       <c r="S7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T7" s="6"/>
+      <c r="T7" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
@@ -1339,7 +1413,7 @@
       <c r="AO7" s="6"/>
       <c r="AP7" s="6"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1397,7 +1471,9 @@
       <c r="S8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T8" s="6"/>
+      <c r="T8" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -1421,7 +1497,7 @@
       <c r="AO8" s="6"/>
       <c r="AP8" s="6"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>73</v>
       </c>
@@ -1479,7 +1555,9 @@
       <c r="S9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T9" s="6"/>
+      <c r="T9" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -1503,7 +1581,7 @@
       <c r="AO9" s="6"/>
       <c r="AP9" s="6"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1561,7 +1639,9 @@
       <c r="S10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T10" s="6"/>
+      <c r="T10" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
@@ -1585,7 +1665,7 @@
       <c r="AO10" s="6"/>
       <c r="AP10" s="6"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
@@ -1641,7 +1721,9 @@
       <c r="S11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T11" s="6"/>
+      <c r="T11" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
@@ -1665,7 +1747,7 @@
       <c r="AO11" s="6"/>
       <c r="AP11" s="6"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1723,7 +1805,9 @@
       <c r="S12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T12" s="6"/>
+      <c r="T12" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
@@ -1747,7 +1831,7 @@
       <c r="AO12" s="6"/>
       <c r="AP12" s="6"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
@@ -1805,7 +1889,9 @@
       <c r="S13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T13" s="6"/>
+      <c r="T13" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
@@ -1829,7 +1915,7 @@
       <c r="AO13" s="6"/>
       <c r="AP13" s="6"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1885,7 +1971,9 @@
       <c r="S14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T14" s="6"/>
+      <c r="T14" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -1909,7 +1997,7 @@
       <c r="AO14" s="6"/>
       <c r="AP14" s="6"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
@@ -1965,7 +2053,9 @@
       <c r="S15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T15" s="6"/>
+      <c r="T15" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
@@ -1989,7 +2079,7 @@
       <c r="AO15" s="6"/>
       <c r="AP15" s="6"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
@@ -2045,7 +2135,9 @@
       <c r="S16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T16" s="6"/>
+      <c r="T16" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
@@ -2069,7 +2161,7 @@
       <c r="AO16" s="6"/>
       <c r="AP16" s="6"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -2125,7 +2217,9 @@
       <c r="S17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T17" s="6"/>
+      <c r="T17" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
@@ -2149,7 +2243,7 @@
       <c r="AO17" s="6"/>
       <c r="AP17" s="6"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>85</v>
       </c>
@@ -2205,7 +2299,9 @@
       <c r="S18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T18" s="6"/>
+      <c r="T18" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
@@ -2229,7 +2325,7 @@
       <c r="AO18" s="6"/>
       <c r="AP18" s="6"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -2287,7 +2383,9 @@
       <c r="S19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T19" s="6"/>
+      <c r="T19" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
@@ -2311,7 +2409,7 @@
       <c r="AO19" s="6"/>
       <c r="AP19" s="6"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -2367,7 +2465,9 @@
       <c r="S20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T20" s="6"/>
+      <c r="T20" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
@@ -2391,7 +2491,7 @@
       <c r="AO20" s="6"/>
       <c r="AP20" s="6"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -2447,7 +2547,9 @@
       <c r="S21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T21" s="6"/>
+      <c r="T21" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
@@ -2471,7 +2573,7 @@
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -2527,7 +2629,9 @@
       <c r="S22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T22" s="6"/>
+      <c r="T22" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
@@ -2551,7 +2655,7 @@
       <c r="AO22" s="6"/>
       <c r="AP22" s="6"/>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>55</v>
       </c>
@@ -2609,7 +2713,9 @@
       <c r="S23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T23" s="6"/>
+      <c r="T23" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
@@ -2633,7 +2739,7 @@
       <c r="AO23" s="6"/>
       <c r="AP23" s="6"/>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
@@ -2689,7 +2795,9 @@
       <c r="S24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T24" s="6"/>
+      <c r="T24" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
@@ -2713,7 +2821,7 @@
       <c r="AO24" s="6"/>
       <c r="AP24" s="6"/>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>57</v>
       </c>
@@ -2771,7 +2879,9 @@
       <c r="S25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T25" s="6"/>
+      <c r="T25" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
@@ -2795,7 +2905,7 @@
       <c r="AO25" s="6"/>
       <c r="AP25" s="6"/>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
@@ -2851,7 +2961,9 @@
       <c r="S26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T26" s="6"/>
+      <c r="T26" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
@@ -2875,7 +2987,7 @@
       <c r="AO26" s="6"/>
       <c r="AP26" s="6"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
@@ -2931,7 +3043,9 @@
       <c r="S27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T27" s="6"/>
+      <c r="T27" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
@@ -2955,7 +3069,7 @@
       <c r="AO27" s="6"/>
       <c r="AP27" s="6"/>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
@@ -3011,7 +3125,9 @@
       <c r="S28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T28" s="6"/>
+      <c r="T28" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
@@ -3035,7 +3151,7 @@
       <c r="AO28" s="6"/>
       <c r="AP28" s="6"/>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
@@ -3091,7 +3207,9 @@
       <c r="S29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T29" s="6"/>
+      <c r="T29" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
@@ -3115,7 +3233,7 @@
       <c r="AO29" s="6"/>
       <c r="AP29" s="6"/>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>62</v>
       </c>
@@ -3171,7 +3289,9 @@
       <c r="S30" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T30" s="6"/>
+      <c r="T30" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
@@ -3195,7 +3315,7 @@
       <c r="AO30" s="6"/>
       <c r="AP30" s="6"/>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>63</v>
       </c>
@@ -3323,7 +3443,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
         <v>64</v>
       </c>
@@ -3379,7 +3499,9 @@
       <c r="S32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T32" s="6"/>
+      <c r="T32" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
       <c r="W32" s="6"/>
@@ -3403,7 +3525,7 @@
       <c r="AO32" s="6"/>
       <c r="AP32" s="6"/>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>65</v>
       </c>
@@ -3459,7 +3581,9 @@
       <c r="S33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T33" s="6"/>
+      <c r="T33" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
       <c r="W33" s="6"/>
@@ -3483,7 +3607,7 @@
       <c r="AO33" s="6"/>
       <c r="AP33" s="6"/>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>66</v>
       </c>
@@ -3611,7 +3735,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>67</v>
       </c>
@@ -3667,7 +3791,9 @@
       <c r="S35" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T35" s="6"/>
+      <c r="T35" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
       <c r="W35" s="6"/>
@@ -3691,7 +3817,7 @@
       <c r="AO35" s="6"/>
       <c r="AP35" s="6"/>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
         <v>68</v>
       </c>
@@ -3747,7 +3873,9 @@
       <c r="S36" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T36" s="6"/>
+      <c r="T36" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
       <c r="W36" s="6"/>
@@ -3771,7 +3899,7 @@
       <c r="AO36" s="6"/>
       <c r="AP36" s="6"/>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.45">
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -3816,16 +3944,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FIX: introduces missing S_DOTNUM state in lexical scanner.
</commit_message>
<xml_diff>
--- a/docs/lexer-FSM.xlsx
+++ b/docs/lexer-FSM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26903664-7424-47E4-A237-C534825D9C6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B321AB6B-D074-4F5E-B479-3CB3C939BDE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="95">
   <si>
     <t>S_START</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>T_PERCENT</t>
+  </si>
+  <si>
+    <t>S_DOTNUM</t>
+  </si>
+  <si>
+    <t>T_FLOAT</t>
   </si>
 </sst>
 </file>
@@ -761,11 +767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP37"/>
+  <dimension ref="A1:AQ36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T36" sqref="T36"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -780,10 +786,13 @@
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="8.06640625" customWidth="1"/>
     <col min="18" max="18" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="19" max="42" width="8.06640625" customWidth="1"/>
+    <col min="19" max="20" width="8.06640625" customWidth="1"/>
+    <col min="21" max="22" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="24" max="43" width="8.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:43" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -843,73 +852,76 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>39</v>
       </c>
@@ -970,7 +982,9 @@
       <c r="T2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U2" s="6"/>
+      <c r="U2" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
@@ -992,8 +1006,9 @@
       <c r="AN2" s="6"/>
       <c r="AO2" s="6"/>
       <c r="AP2" s="6"/>
+      <c r="AQ2" s="6"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -1054,7 +1069,9 @@
       <c r="T3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="6"/>
+      <c r="U3" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
@@ -1076,8 +1093,9 @@
       <c r="AN3" s="6"/>
       <c r="AO3" s="6"/>
       <c r="AP3" s="6"/>
+      <c r="AQ3" s="6"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
@@ -1138,8 +1156,12 @@
       <c r="T4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
+      <c r="U4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
@@ -1160,8 +1182,9 @@
       <c r="AN4" s="6"/>
       <c r="AO4" s="6"/>
       <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
@@ -1222,8 +1245,12 @@
       <c r="T5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
+      <c r="U5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
@@ -1244,8 +1271,9 @@
       <c r="AN5" s="6"/>
       <c r="AO5" s="6"/>
       <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -1306,7 +1334,9 @@
       <c r="T6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U6" s="6"/>
+      <c r="U6" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
@@ -1328,8 +1358,9 @@
       <c r="AN6" s="6"/>
       <c r="AO6" s="6"/>
       <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>44</v>
       </c>
@@ -1390,7 +1421,9 @@
       <c r="T7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U7" s="6"/>
+      <c r="U7" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
@@ -1412,8 +1445,9 @@
       <c r="AN7" s="6"/>
       <c r="AO7" s="6"/>
       <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1474,7 +1508,9 @@
       <c r="T8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U8" s="6"/>
+      <c r="U8" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
@@ -1496,8 +1532,9 @@
       <c r="AN8" s="6"/>
       <c r="AO8" s="6"/>
       <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>73</v>
       </c>
@@ -1558,7 +1595,9 @@
       <c r="T9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U9" s="6"/>
+      <c r="U9" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
@@ -1580,8 +1619,9 @@
       <c r="AN9" s="6"/>
       <c r="AO9" s="6"/>
       <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1642,7 +1682,9 @@
       <c r="T10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U10" s="6"/>
+      <c r="U10" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
@@ -1664,8 +1706,9 @@
       <c r="AN10" s="6"/>
       <c r="AO10" s="6"/>
       <c r="AP10" s="6"/>
+      <c r="AQ10" s="6"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1767,9 @@
       <c r="T11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U11" s="6"/>
+      <c r="U11" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
@@ -1746,8 +1791,9 @@
       <c r="AN11" s="6"/>
       <c r="AO11" s="6"/>
       <c r="AP11" s="6"/>
+      <c r="AQ11" s="6"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1808,7 +1854,9 @@
       <c r="T12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U12" s="6"/>
+      <c r="U12" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
@@ -1830,8 +1878,9 @@
       <c r="AN12" s="6"/>
       <c r="AO12" s="6"/>
       <c r="AP12" s="6"/>
+      <c r="AQ12" s="6"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
@@ -1892,8 +1941,9 @@
       <c r="T13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
+      <c r="U13" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
@@ -1914,8 +1964,9 @@
       <c r="AN13" s="6"/>
       <c r="AO13" s="6"/>
       <c r="AP13" s="6"/>
+      <c r="AQ13" s="6"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1974,7 +2025,9 @@
       <c r="T14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="U14" s="6"/>
+      <c r="U14" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
@@ -1996,8 +2049,9 @@
       <c r="AN14" s="6"/>
       <c r="AO14" s="6"/>
       <c r="AP14" s="6"/>
+      <c r="AQ14" s="6"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
@@ -2056,7 +2110,9 @@
       <c r="T15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U15" s="6"/>
+      <c r="U15" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
@@ -2078,8 +2134,9 @@
       <c r="AN15" s="6"/>
       <c r="AO15" s="6"/>
       <c r="AP15" s="6"/>
+      <c r="AQ15" s="6"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
@@ -2138,8 +2195,9 @@
       <c r="T16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
+      <c r="U16" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
@@ -2160,8 +2218,9 @@
       <c r="AN16" s="6"/>
       <c r="AO16" s="6"/>
       <c r="AP16" s="6"/>
+      <c r="AQ16" s="6"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -2220,8 +2279,12 @@
       <c r="T17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
+      <c r="U17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
@@ -2242,8 +2305,9 @@
       <c r="AN17" s="6"/>
       <c r="AO17" s="6"/>
       <c r="AP17" s="6"/>
+      <c r="AQ17" s="6"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>85</v>
       </c>
@@ -2302,7 +2366,9 @@
       <c r="T18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U18" s="6"/>
+      <c r="U18" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
@@ -2324,8 +2390,9 @@
       <c r="AN18" s="6"/>
       <c r="AO18" s="6"/>
       <c r="AP18" s="6"/>
+      <c r="AQ18" s="6"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -2386,7 +2453,9 @@
       <c r="T19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U19" s="6"/>
+      <c r="U19" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
@@ -2408,8 +2477,9 @@
       <c r="AN19" s="6"/>
       <c r="AO19" s="6"/>
       <c r="AP19" s="6"/>
+      <c r="AQ19" s="6"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -2468,7 +2538,9 @@
       <c r="T20" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U20" s="6"/>
+      <c r="U20" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
@@ -2490,8 +2562,9 @@
       <c r="AN20" s="6"/>
       <c r="AO20" s="6"/>
       <c r="AP20" s="6"/>
+      <c r="AQ20" s="6"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
@@ -2550,7 +2623,9 @@
       <c r="T21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U21" s="6"/>
+      <c r="U21" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
@@ -2572,8 +2647,9 @@
       <c r="AN21" s="6"/>
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
+      <c r="AQ21" s="6"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -2632,7 +2708,9 @@
       <c r="T22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U22" s="6"/>
+      <c r="U22" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
@@ -2654,8 +2732,9 @@
       <c r="AN22" s="6"/>
       <c r="AO22" s="6"/>
       <c r="AP22" s="6"/>
+      <c r="AQ22" s="6"/>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>55</v>
       </c>
@@ -2716,8 +2795,12 @@
       <c r="T23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
+      <c r="U23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
@@ -2738,8 +2821,9 @@
       <c r="AN23" s="6"/>
       <c r="AO23" s="6"/>
       <c r="AP23" s="6"/>
+      <c r="AQ23" s="6"/>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
@@ -2798,7 +2882,9 @@
       <c r="T24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="U24" s="6"/>
+      <c r="U24" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
@@ -2820,8 +2906,9 @@
       <c r="AN24" s="6"/>
       <c r="AO24" s="6"/>
       <c r="AP24" s="6"/>
+      <c r="AQ24" s="6"/>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>57</v>
       </c>
@@ -2882,7 +2969,9 @@
       <c r="T25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U25" s="6"/>
+      <c r="U25" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
@@ -2904,8 +2993,9 @@
       <c r="AN25" s="6"/>
       <c r="AO25" s="6"/>
       <c r="AP25" s="6"/>
+      <c r="AQ25" s="6"/>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
@@ -2964,7 +3054,9 @@
       <c r="T26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="U26" s="6"/>
+      <c r="U26" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
@@ -2986,8 +3078,9 @@
       <c r="AN26" s="6"/>
       <c r="AO26" s="6"/>
       <c r="AP26" s="6"/>
+      <c r="AQ26" s="6"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
@@ -3044,10 +3137,14 @@
         <v>13</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
+        <v>93</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="V27" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
       <c r="Y27" s="6"/>
@@ -3068,8 +3165,9 @@
       <c r="AN27" s="6"/>
       <c r="AO27" s="6"/>
       <c r="AP27" s="6"/>
+      <c r="AQ27" s="6"/>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
@@ -3128,7 +3226,9 @@
       <c r="T28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U28" s="6"/>
+      <c r="U28" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
@@ -3150,8 +3250,9 @@
       <c r="AN28" s="6"/>
       <c r="AO28" s="6"/>
       <c r="AP28" s="6"/>
+      <c r="AQ28" s="6"/>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
@@ -3210,7 +3311,9 @@
       <c r="T29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U29" s="6"/>
+      <c r="U29" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
       <c r="X29" s="6"/>
@@ -3232,8 +3335,9 @@
       <c r="AN29" s="6"/>
       <c r="AO29" s="6"/>
       <c r="AP29" s="6"/>
+      <c r="AQ29" s="6"/>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>62</v>
       </c>
@@ -3292,7 +3396,9 @@
       <c r="T30" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U30" s="6"/>
+      <c r="U30" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
@@ -3314,138 +3420,96 @@
       <c r="AN30" s="6"/>
       <c r="AO30" s="6"/>
       <c r="AP30" s="6"/>
+      <c r="AQ30" s="6"/>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="U31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="W31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AN31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP31" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+      <c r="AA31" s="6"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="6"/>
+      <c r="AG31" s="6"/>
+      <c r="AH31" s="6"/>
+      <c r="AI31" s="6"/>
+      <c r="AJ31" s="6"/>
+      <c r="AK31" s="6"/>
+      <c r="AL31" s="6"/>
+      <c r="AM31" s="6"/>
+      <c r="AN31" s="6"/>
+      <c r="AO31" s="6"/>
+      <c r="AP31" s="6"/>
+      <c r="AQ31" s="6"/>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
@@ -3502,7 +3566,9 @@
       <c r="T32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U32" s="6"/>
+      <c r="U32" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V32" s="6"/>
       <c r="W32" s="6"/>
       <c r="X32" s="6"/>
@@ -3524,10 +3590,11 @@
       <c r="AN32" s="6"/>
       <c r="AO32" s="6"/>
       <c r="AP32" s="6"/>
+      <c r="AQ32" s="6"/>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
@@ -3584,7 +3651,9 @@
       <c r="T33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="U33" s="6"/>
+      <c r="U33" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="V33" s="6"/>
       <c r="W33" s="6"/>
       <c r="X33" s="6"/>
@@ -3606,341 +3675,354 @@
       <c r="AN33" s="6"/>
       <c r="AO33" s="6"/>
       <c r="AP33" s="6"/>
+      <c r="AQ33" s="6"/>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="6"/>
+      <c r="AB34" s="6"/>
+      <c r="AC34" s="6"/>
+      <c r="AD34" s="6"/>
+      <c r="AE34" s="6"/>
+      <c r="AF34" s="6"/>
+      <c r="AG34" s="6"/>
+      <c r="AH34" s="6"/>
+      <c r="AI34" s="6"/>
+      <c r="AJ34" s="6"/>
+      <c r="AK34" s="6"/>
+      <c r="AL34" s="6"/>
+      <c r="AM34" s="6"/>
+      <c r="AN34" s="6"/>
+      <c r="AO34" s="6"/>
+      <c r="AP34" s="6"/>
+      <c r="AQ34" s="6"/>
+    </row>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A35" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="L34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="O34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="P34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="R34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="S34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="T34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="U34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="V34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="X34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP34" s="7" t="s">
+      <c r="B35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="R35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ35" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.45">
-      <c r="A35" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R35" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="S35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="T35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="U35" s="6"/>
-      <c r="V35" s="6"/>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="6"/>
-      <c r="Z35" s="6"/>
-      <c r="AA35" s="6"/>
-      <c r="AB35" s="6"/>
-      <c r="AC35" s="6"/>
-      <c r="AD35" s="6"/>
-      <c r="AE35" s="6"/>
-      <c r="AF35" s="6"/>
-      <c r="AG35" s="6"/>
-      <c r="AH35" s="6"/>
-      <c r="AI35" s="6"/>
-      <c r="AJ35" s="6"/>
-      <c r="AK35" s="6"/>
-      <c r="AL35" s="6"/>
-      <c r="AM35" s="6"/>
-      <c r="AN35" s="6"/>
-      <c r="AO35" s="6"/>
-      <c r="AP35" s="6"/>
-    </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N36" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R36" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="S36" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="T36" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="6"/>
-      <c r="AE36" s="6"/>
-      <c r="AF36" s="6"/>
-      <c r="AG36" s="6"/>
-      <c r="AH36" s="6"/>
-      <c r="AI36" s="6"/>
-      <c r="AJ36" s="6"/>
-      <c r="AK36" s="6"/>
-      <c r="AL36" s="6"/>
-      <c r="AM36" s="6"/>
-      <c r="AN36" s="6"/>
-      <c r="AO36" s="6"/>
-      <c r="AP36" s="6"/>
-    </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.45">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
-      <c r="U37" s="6"/>
-      <c r="V37" s="6"/>
-      <c r="W37" s="6"/>
-      <c r="X37" s="6"/>
-      <c r="Y37" s="6"/>
-      <c r="Z37" s="6"/>
-      <c r="AA37" s="6"/>
-      <c r="AB37" s="6"/>
-      <c r="AC37" s="6"/>
-      <c r="AD37" s="6"/>
-      <c r="AE37" s="6"/>
-      <c r="AF37" s="6"/>
-      <c r="AG37" s="6"/>
-      <c r="AH37" s="6"/>
-      <c r="AI37" s="6"/>
-      <c r="AJ37" s="6"/>
-      <c r="AK37" s="6"/>
-      <c r="AL37" s="6"/>
-      <c r="AM37" s="6"/>
-      <c r="AN37" s="6"/>
-      <c r="AO37" s="6"/>
-      <c r="AP37" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AN36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ36" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FEAT: fills fully the lexical scanner transitions table.
</commit_message>
<xml_diff>
--- a/docs/lexer-FSM.xlsx
+++ b/docs/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B321AB6B-D074-4F5E-B479-3CB3C939BDE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="Transitions" sheetId="2" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="105">
   <si>
     <t>S_START</t>
   </si>
@@ -306,13 +300,43 @@
   </si>
   <si>
     <t>T_FLOAT</t>
+  </si>
+  <si>
+    <t>T_TUPLE</t>
+  </si>
+  <si>
+    <t>T_DATE</t>
+  </si>
+  <si>
+    <t>T_TIME</t>
+  </si>
+  <si>
+    <t>T_PAIR</t>
+  </si>
+  <si>
+    <t>T_TAG</t>
+  </si>
+  <si>
+    <t>T_MONEY</t>
+  </si>
+  <si>
+    <t>T_URL</t>
+  </si>
+  <si>
+    <t>T_PATH</t>
+  </si>
+  <si>
+    <t>S_WORDSET</t>
+  </si>
+  <si>
+    <t>T_EMAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +371,12 @@
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -427,6 +457,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -489,7 +522,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,26 +555,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,23 +590,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -766,33 +765,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L37" sqref="L37"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL41" sqref="AL41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" customWidth="1"/>
-    <col min="2" max="6" width="8.06640625" customWidth="1"/>
-    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.06640625" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.06640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.08984375" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.08984375" customWidth="1"/>
+    <col min="13" max="13" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.08984375" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.06640625" customWidth="1"/>
-    <col min="18" max="18" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.06640625" customWidth="1"/>
-    <col min="21" max="22" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="24" max="43" width="8.06640625" customWidth="1"/>
+    <col min="16" max="17" width="8.08984375" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.08984375" customWidth="1"/>
+    <col min="21" max="22" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="30" width="8.08984375" customWidth="1"/>
+    <col min="31" max="31" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="33" max="36" width="8.08984375" customWidth="1"/>
+    <col min="37" max="38" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="8.08984375" customWidth="1"/>
+    <col min="41" max="41" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="8.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -878,41 +885,41 @@
       <c r="AC1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="AG1" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="AH1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="AP1" s="2" t="s">
         <v>35</v>
@@ -921,7 +928,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>39</v>
       </c>
@@ -985,30 +992,74 @@
       <c r="U2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
-      <c r="AM2" s="6"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="6"/>
-      <c r="AQ2" s="6"/>
+      <c r="V2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -1072,30 +1123,74 @@
       <c r="U3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="6"/>
-      <c r="AQ3" s="6"/>
+      <c r="V3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
@@ -1162,29 +1257,71 @@
       <c r="V4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="6"/>
-      <c r="AL4" s="6"/>
-      <c r="AM4" s="6"/>
-      <c r="AN4" s="6"/>
-      <c r="AO4" s="6"/>
-      <c r="AP4" s="6"/>
-      <c r="AQ4" s="6"/>
+      <c r="W4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ4" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
@@ -1251,29 +1388,71 @@
       <c r="V5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
-      <c r="AM5" s="6"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="6"/>
-      <c r="AQ5" s="6"/>
+      <c r="W5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ5" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -1337,30 +1516,74 @@
       <c r="U6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
-      <c r="AG6" s="6"/>
-      <c r="AH6" s="6"/>
-      <c r="AI6" s="6"/>
-      <c r="AJ6" s="6"/>
-      <c r="AK6" s="6"/>
-      <c r="AL6" s="6"/>
-      <c r="AM6" s="6"/>
-      <c r="AN6" s="6"/>
-      <c r="AO6" s="6"/>
-      <c r="AP6" s="6"/>
-      <c r="AQ6" s="6"/>
+      <c r="V6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>44</v>
       </c>
@@ -1424,30 +1647,74 @@
       <c r="U7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
-      <c r="AG7" s="6"/>
-      <c r="AH7" s="6"/>
-      <c r="AI7" s="6"/>
-      <c r="AJ7" s="6"/>
-      <c r="AK7" s="6"/>
-      <c r="AL7" s="6"/>
-      <c r="AM7" s="6"/>
-      <c r="AN7" s="6"/>
-      <c r="AO7" s="6"/>
-      <c r="AP7" s="6"/>
-      <c r="AQ7" s="6"/>
+      <c r="V7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1511,30 +1778,74 @@
       <c r="U8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-      <c r="AI8" s="6"/>
-      <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
-      <c r="AL8" s="6"/>
-      <c r="AM8" s="6"/>
-      <c r="AN8" s="6"/>
-      <c r="AO8" s="6"/>
-      <c r="AP8" s="6"/>
-      <c r="AQ8" s="6"/>
+      <c r="V8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ8" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>73</v>
       </c>
@@ -1598,30 +1909,74 @@
       <c r="U9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
-      <c r="AG9" s="6"/>
-      <c r="AH9" s="6"/>
-      <c r="AI9" s="6"/>
-      <c r="AJ9" s="6"/>
-      <c r="AK9" s="6"/>
-      <c r="AL9" s="6"/>
-      <c r="AM9" s="6"/>
-      <c r="AN9" s="6"/>
-      <c r="AO9" s="6"/>
-      <c r="AP9" s="6"/>
-      <c r="AQ9" s="6"/>
+      <c r="V9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1685,34 +2040,80 @@
       <c r="U10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6"/>
-      <c r="AI10" s="6"/>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="6"/>
-      <c r="AL10" s="6"/>
-      <c r="AM10" s="6"/>
-      <c r="AN10" s="6"/>
-      <c r="AO10" s="6"/>
-      <c r="AP10" s="6"/>
-      <c r="AQ10" s="6"/>
+      <c r="V10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="C11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1770,30 +2171,74 @@
       <c r="U11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="6"/>
-      <c r="AH11" s="6"/>
-      <c r="AI11" s="6"/>
-      <c r="AJ11" s="6"/>
-      <c r="AK11" s="6"/>
-      <c r="AL11" s="6"/>
-      <c r="AM11" s="6"/>
-      <c r="AN11" s="6"/>
-      <c r="AO11" s="6"/>
-      <c r="AP11" s="6"/>
-      <c r="AQ11" s="6"/>
+      <c r="V11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ11" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1857,30 +2302,74 @@
       <c r="U12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="6"/>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="6"/>
-      <c r="AL12" s="6"/>
-      <c r="AM12" s="6"/>
-      <c r="AN12" s="6"/>
-      <c r="AO12" s="6"/>
-      <c r="AP12" s="6"/>
-      <c r="AQ12" s="6"/>
+      <c r="V12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ12" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:43" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
@@ -1944,33 +2433,80 @@
       <c r="U13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="6"/>
-      <c r="AH13" s="6"/>
-      <c r="AI13" s="6"/>
-      <c r="AJ13" s="6"/>
-      <c r="AK13" s="6"/>
-      <c r="AL13" s="6"/>
-      <c r="AM13" s="6"/>
-      <c r="AN13" s="6"/>
-      <c r="AO13" s="6"/>
-      <c r="AP13" s="6"/>
-      <c r="AQ13" s="6"/>
+      <c r="V13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ13" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C14" s="6" t="s">
         <v>0</v>
       </c>
@@ -2028,34 +2564,80 @@
       <c r="U14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
-      <c r="AL14" s="6"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
-      <c r="AO14" s="6"/>
-      <c r="AP14" s="6"/>
-      <c r="AQ14" s="6"/>
+      <c r="V14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ14" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C15" s="6" t="s">
         <v>0</v>
       </c>
@@ -2113,34 +2695,80 @@
       <c r="U15" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="6"/>
-      <c r="AG15" s="6"/>
-      <c r="AH15" s="6"/>
-      <c r="AI15" s="6"/>
-      <c r="AJ15" s="6"/>
-      <c r="AK15" s="6"/>
-      <c r="AL15" s="6"/>
-      <c r="AM15" s="6"/>
-      <c r="AN15" s="6"/>
-      <c r="AO15" s="6"/>
-      <c r="AP15" s="6"/>
-      <c r="AQ15" s="6"/>
+      <c r="V15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AO15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ15" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C16" s="6" t="s">
         <v>0</v>
       </c>
@@ -2198,33 +2826,80 @@
       <c r="U16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
-      <c r="AG16" s="6"/>
-      <c r="AH16" s="6"/>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
-      <c r="AL16" s="6"/>
-      <c r="AM16" s="6"/>
-      <c r="AN16" s="6"/>
-      <c r="AO16" s="6"/>
-      <c r="AP16" s="6"/>
-      <c r="AQ16" s="6"/>
+      <c r="V16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ16" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="6" t="s">
         <v>0</v>
       </c>
@@ -2285,33 +2960,77 @@
       <c r="V17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="6"/>
-      <c r="AG17" s="6"/>
-      <c r="AH17" s="6"/>
-      <c r="AI17" s="6"/>
-      <c r="AJ17" s="6"/>
-      <c r="AK17" s="6"/>
-      <c r="AL17" s="6"/>
-      <c r="AM17" s="6"/>
-      <c r="AN17" s="6"/>
-      <c r="AO17" s="6"/>
-      <c r="AP17" s="6"/>
-      <c r="AQ17" s="6"/>
+      <c r="W17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ17" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C18" s="6" t="s">
         <v>0</v>
       </c>
@@ -2369,30 +3088,74 @@
       <c r="U18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18" s="6"/>
-      <c r="AG18" s="6"/>
-      <c r="AH18" s="6"/>
-      <c r="AI18" s="6"/>
-      <c r="AJ18" s="6"/>
-      <c r="AK18" s="6"/>
-      <c r="AL18" s="6"/>
-      <c r="AM18" s="6"/>
-      <c r="AN18" s="6"/>
-      <c r="AO18" s="6"/>
-      <c r="AP18" s="6"/>
-      <c r="AQ18" s="6"/>
+      <c r="V18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ18" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -2456,34 +3219,80 @@
       <c r="U19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="6"/>
-      <c r="AF19" s="6"/>
-      <c r="AG19" s="6"/>
-      <c r="AH19" s="6"/>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
-      <c r="AL19" s="6"/>
-      <c r="AM19" s="6"/>
-      <c r="AN19" s="6"/>
-      <c r="AO19" s="6"/>
-      <c r="AP19" s="6"/>
-      <c r="AQ19" s="6"/>
+      <c r="V19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ19" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="C20" s="6" t="s">
         <v>0</v>
       </c>
@@ -2541,34 +3350,80 @@
       <c r="U20" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="6"/>
-      <c r="AG20" s="6"/>
-      <c r="AH20" s="6"/>
-      <c r="AI20" s="6"/>
-      <c r="AJ20" s="6"/>
-      <c r="AK20" s="6"/>
-      <c r="AL20" s="6"/>
-      <c r="AM20" s="6"/>
-      <c r="AN20" s="6"/>
-      <c r="AO20" s="6"/>
-      <c r="AP20" s="6"/>
-      <c r="AQ20" s="6"/>
+      <c r="V20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="C21" s="6" t="s">
         <v>0</v>
       </c>
@@ -2626,34 +3481,80 @@
       <c r="U21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
-      <c r="AC21" s="6"/>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="6"/>
-      <c r="AG21" s="6"/>
-      <c r="AH21" s="6"/>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" s="6"/>
-      <c r="AL21" s="6"/>
-      <c r="AM21" s="6"/>
-      <c r="AN21" s="6"/>
-      <c r="AO21" s="6"/>
-      <c r="AP21" s="6"/>
-      <c r="AQ21" s="6"/>
+      <c r="V21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ21" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C22" s="6" t="s">
         <v>0</v>
       </c>
@@ -2711,30 +3612,74 @@
       <c r="U22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
-      <c r="AF22" s="6"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
-      <c r="AL22" s="6"/>
-      <c r="AM22" s="6"/>
-      <c r="AN22" s="6"/>
-      <c r="AO22" s="6"/>
-      <c r="AP22" s="6"/>
-      <c r="AQ22" s="6"/>
+      <c r="V22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ22" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>55</v>
       </c>
@@ -2801,33 +3746,77 @@
       <c r="V23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
-      <c r="AE23" s="6"/>
-      <c r="AF23" s="6"/>
-      <c r="AG23" s="6"/>
-      <c r="AH23" s="6"/>
-      <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="6"/>
-      <c r="AM23" s="6"/>
-      <c r="AN23" s="6"/>
-      <c r="AO23" s="6"/>
-      <c r="AP23" s="6"/>
-      <c r="AQ23" s="6"/>
+      <c r="W23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ23" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="C24" s="6" t="s">
         <v>0</v>
       </c>
@@ -2885,30 +3874,74 @@
       <c r="U24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
-      <c r="AI24" s="6"/>
-      <c r="AJ24" s="6"/>
-      <c r="AK24" s="6"/>
-      <c r="AL24" s="6"/>
-      <c r="AM24" s="6"/>
-      <c r="AN24" s="6"/>
-      <c r="AO24" s="6"/>
-      <c r="AP24" s="6"/>
-      <c r="AQ24" s="6"/>
+      <c r="V24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ24" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>57</v>
       </c>
@@ -2972,34 +4005,80 @@
       <c r="U25" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-      <c r="AA25" s="6"/>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
-      <c r="AD25" s="6"/>
-      <c r="AE25" s="6"/>
-      <c r="AF25" s="6"/>
-      <c r="AG25" s="6"/>
-      <c r="AH25" s="6"/>
-      <c r="AI25" s="6"/>
-      <c r="AJ25" s="6"/>
-      <c r="AK25" s="6"/>
-      <c r="AL25" s="6"/>
-      <c r="AM25" s="6"/>
-      <c r="AN25" s="6"/>
-      <c r="AO25" s="6"/>
-      <c r="AP25" s="6"/>
-      <c r="AQ25" s="6"/>
+      <c r="V25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ25" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="C26" s="6" t="s">
         <v>0</v>
       </c>
@@ -3057,34 +4136,80 @@
       <c r="U26" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
-      <c r="AC26" s="6"/>
-      <c r="AD26" s="6"/>
-      <c r="AE26" s="6"/>
-      <c r="AF26" s="6"/>
-      <c r="AG26" s="6"/>
-      <c r="AH26" s="6"/>
-      <c r="AI26" s="6"/>
-      <c r="AJ26" s="6"/>
-      <c r="AK26" s="6"/>
-      <c r="AL26" s="6"/>
-      <c r="AM26" s="6"/>
-      <c r="AN26" s="6"/>
-      <c r="AO26" s="6"/>
-      <c r="AP26" s="6"/>
-      <c r="AQ26" s="6"/>
+      <c r="V26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ26" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C27" s="6" t="s">
         <v>0</v>
       </c>
@@ -3145,33 +4270,77 @@
       <c r="V27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="6"/>
-      <c r="AD27" s="6"/>
-      <c r="AE27" s="6"/>
-      <c r="AF27" s="6"/>
-      <c r="AG27" s="6"/>
-      <c r="AH27" s="6"/>
-      <c r="AI27" s="6"/>
-      <c r="AJ27" s="6"/>
-      <c r="AK27" s="6"/>
-      <c r="AL27" s="6"/>
-      <c r="AM27" s="6"/>
-      <c r="AN27" s="6"/>
-      <c r="AO27" s="6"/>
-      <c r="AP27" s="6"/>
-      <c r="AQ27" s="6"/>
+      <c r="W27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ27" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="C28" s="6" t="s">
         <v>0</v>
       </c>
@@ -3229,34 +4398,80 @@
       <c r="U28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="6"/>
-      <c r="AA28" s="6"/>
-      <c r="AB28" s="6"/>
-      <c r="AC28" s="6"/>
-      <c r="AD28" s="6"/>
-      <c r="AE28" s="6"/>
-      <c r="AF28" s="6"/>
-      <c r="AG28" s="6"/>
-      <c r="AH28" s="6"/>
-      <c r="AI28" s="6"/>
-      <c r="AJ28" s="6"/>
-      <c r="AK28" s="6"/>
-      <c r="AL28" s="6"/>
-      <c r="AM28" s="6"/>
-      <c r="AN28" s="6"/>
-      <c r="AO28" s="6"/>
-      <c r="AP28" s="6"/>
-      <c r="AQ28" s="6"/>
+      <c r="V28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ28" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="C29" s="6" t="s">
         <v>0</v>
       </c>
@@ -3314,34 +4529,80 @@
       <c r="U29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6"/>
-      <c r="AA29" s="6"/>
-      <c r="AB29" s="6"/>
-      <c r="AC29" s="6"/>
-      <c r="AD29" s="6"/>
-      <c r="AE29" s="6"/>
-      <c r="AF29" s="6"/>
-      <c r="AG29" s="6"/>
-      <c r="AH29" s="6"/>
-      <c r="AI29" s="6"/>
-      <c r="AJ29" s="6"/>
-      <c r="AK29" s="6"/>
-      <c r="AL29" s="6"/>
-      <c r="AM29" s="6"/>
-      <c r="AN29" s="6"/>
-      <c r="AO29" s="6"/>
-      <c r="AP29" s="6"/>
-      <c r="AQ29" s="6"/>
+      <c r="V29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM29" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN29" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO29" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ29" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
@@ -3399,34 +4660,80 @@
       <c r="U30" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="6"/>
-      <c r="AB30" s="6"/>
-      <c r="AC30" s="6"/>
-      <c r="AD30" s="6"/>
-      <c r="AE30" s="6"/>
-      <c r="AF30" s="6"/>
-      <c r="AG30" s="6"/>
-      <c r="AH30" s="6"/>
-      <c r="AI30" s="6"/>
-      <c r="AJ30" s="6"/>
-      <c r="AK30" s="6"/>
-      <c r="AL30" s="6"/>
-      <c r="AM30" s="6"/>
-      <c r="AN30" s="6"/>
-      <c r="AO30" s="6"/>
-      <c r="AP30" s="6"/>
-      <c r="AQ30" s="6"/>
+      <c r="V30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ30" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C31" s="6" t="s">
         <v>0</v>
       </c>
@@ -3484,34 +4791,80 @@
       <c r="U31" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6"/>
-      <c r="AA31" s="6"/>
-      <c r="AB31" s="6"/>
-      <c r="AC31" s="6"/>
-      <c r="AD31" s="6"/>
-      <c r="AE31" s="6"/>
-      <c r="AF31" s="6"/>
-      <c r="AG31" s="6"/>
-      <c r="AH31" s="6"/>
-      <c r="AI31" s="6"/>
-      <c r="AJ31" s="6"/>
-      <c r="AK31" s="6"/>
-      <c r="AL31" s="6"/>
-      <c r="AM31" s="6"/>
-      <c r="AN31" s="6"/>
-      <c r="AO31" s="6"/>
-      <c r="AP31" s="6"/>
-      <c r="AQ31" s="6"/>
+      <c r="V31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ31" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C32" s="6" t="s">
         <v>0</v>
       </c>
@@ -3569,34 +4922,80 @@
       <c r="U32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="6"/>
-      <c r="AB32" s="6"/>
-      <c r="AC32" s="6"/>
-      <c r="AD32" s="6"/>
-      <c r="AE32" s="6"/>
-      <c r="AF32" s="6"/>
-      <c r="AG32" s="6"/>
-      <c r="AH32" s="6"/>
-      <c r="AI32" s="6"/>
-      <c r="AJ32" s="6"/>
-      <c r="AK32" s="6"/>
-      <c r="AL32" s="6"/>
-      <c r="AM32" s="6"/>
-      <c r="AN32" s="6"/>
-      <c r="AO32" s="6"/>
-      <c r="AP32" s="6"/>
-      <c r="AQ32" s="6"/>
+      <c r="V32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ32" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="6"/>
+      <c r="B33" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C33" s="6" t="s">
         <v>0</v>
       </c>
@@ -3654,34 +5053,80 @@
       <c r="U33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="6"/>
-      <c r="AE33" s="6"/>
-      <c r="AF33" s="6"/>
-      <c r="AG33" s="6"/>
-      <c r="AH33" s="6"/>
-      <c r="AI33" s="6"/>
-      <c r="AJ33" s="6"/>
-      <c r="AK33" s="6"/>
-      <c r="AL33" s="6"/>
-      <c r="AM33" s="6"/>
-      <c r="AN33" s="6"/>
-      <c r="AO33" s="6"/>
-      <c r="AP33" s="6"/>
-      <c r="AQ33" s="6"/>
+      <c r="V33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO33" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ33" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C34" s="6" t="s">
         <v>0</v>
       </c>
@@ -3739,30 +5184,74 @@
       <c r="U34" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-      <c r="AA34" s="6"/>
-      <c r="AB34" s="6"/>
-      <c r="AC34" s="6"/>
-      <c r="AD34" s="6"/>
-      <c r="AE34" s="6"/>
-      <c r="AF34" s="6"/>
-      <c r="AG34" s="6"/>
-      <c r="AH34" s="6"/>
-      <c r="AI34" s="6"/>
-      <c r="AJ34" s="6"/>
-      <c r="AK34" s="6"/>
-      <c r="AL34" s="6"/>
-      <c r="AM34" s="6"/>
-      <c r="AN34" s="6"/>
-      <c r="AO34" s="6"/>
-      <c r="AP34" s="6"/>
-      <c r="AQ34" s="6"/>
+      <c r="V34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ34" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>66</v>
       </c>
@@ -3893,7 +5382,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>63</v>
       </c>
@@ -4031,12 +5520,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FEAT: removes C_UCS2 and C_UCS4 classes.
They are replaced by simple flags.
</commit_message>
<xml_diff>
--- a/docs/lexer-FSM.xlsx
+++ b/docs/lexer-FSM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="103">
   <si>
     <t>S_START</t>
   </si>
@@ -209,18 +209,9 @@
     <t>C_EOF</t>
   </si>
   <si>
-    <t>C_UCS2</t>
-  </si>
-  <si>
-    <t>C_UCS4</t>
-  </si>
-  <si>
     <t>C_ILLEGAL</t>
   </si>
   <si>
-    <t>C_NO_OP</t>
-  </si>
-  <si>
     <t>C_WORD</t>
   </si>
   <si>
@@ -330,6 +321,9 @@
   </si>
   <si>
     <t>T_EMAIL</t>
+  </si>
+  <si>
+    <t>C_BIN</t>
   </si>
 </sst>
 </file>
@@ -766,11 +760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ36"/>
+  <dimension ref="A1:AQ34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL41" sqref="AL41"/>
+      <selection pane="topRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,10 +802,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -820,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -841,7 +835,7 @@
         <v>9</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>10</v>
@@ -859,7 +853,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>15</v>
@@ -919,7 +913,7 @@
         <v>34</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AP1" s="2" t="s">
         <v>35</v>
@@ -939,13 +933,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>3</v>
@@ -954,25 +948,25 @@
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>10</v>
@@ -984,49 +978,49 @@
         <v>12</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X2" s="1" t="s">
+      <c r="AB2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AD2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH2" s="6" t="s">
         <v>28</v>
@@ -1047,16 +1041,16 @@
         <v>34</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
@@ -1073,10 +1067,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>3</v>
@@ -1085,19 +1079,19 @@
         <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>9</v>
@@ -1115,49 +1109,49 @@
         <v>12</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" s="1" t="s">
+      <c r="AB3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AD3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH3" s="6" t="s">
         <v>28</v>
@@ -1178,16 +1172,16 @@
         <v>34</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
@@ -1201,13 +1195,13 @@
         <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>3</v>
@@ -1234,7 +1228,7 @@
         <v>9</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>10</v>
@@ -1258,7 +1252,7 @@
         <v>15</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>17</v>
@@ -1332,13 +1326,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>3</v>
@@ -1365,7 +1359,7 @@
         <v>9</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>10</v>
@@ -1389,7 +1383,7 @@
         <v>15</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X5" s="6" t="s">
         <v>17</v>
@@ -1457,19 +1451,19 @@
         <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>3</v>
@@ -1478,25 +1472,25 @@
         <v>3</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>10</v>
@@ -1508,49 +1502,49 @@
         <v>12</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X6" s="1" t="s">
+      <c r="AB6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AD6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH6" s="6" t="s">
         <v>28</v>
@@ -1571,16 +1565,16 @@
         <v>34</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
@@ -1588,19 +1582,19 @@
         <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>3</v>
@@ -1609,25 +1603,25 @@
         <v>3</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>10</v>
@@ -1636,52 +1630,52 @@
         <v>10</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X7" s="1" t="s">
+      <c r="AB7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AD7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE7" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE7" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH7" s="6" t="s">
         <v>28</v>
@@ -1702,16 +1696,16 @@
         <v>34</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ7" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.35">
@@ -1719,19 +1713,19 @@
         <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>3</v>
@@ -1740,25 +1734,25 @@
         <v>3</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>10</v>
@@ -1770,49 +1764,49 @@
         <v>12</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="V8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X8" s="1" t="s">
+      <c r="AB8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AD8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE8" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF8" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH8" s="6" t="s">
         <v>28</v>
@@ -1833,36 +1827,36 @@
         <v>34</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ8" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ8" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>3</v>
@@ -1871,25 +1865,25 @@
         <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>10</v>
@@ -1901,49 +1895,49 @@
         <v>12</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="V9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X9" s="1" t="s">
+      <c r="AB9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AD9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE9" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH9" s="6" t="s">
         <v>28</v>
@@ -1964,16 +1958,16 @@
         <v>34</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO9" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ9" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.35">
@@ -1987,13 +1981,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>3</v>
@@ -2002,25 +1996,25 @@
         <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>10</v>
@@ -2032,49 +2026,49 @@
         <v>12</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X10" s="1" t="s">
+      <c r="AB10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AD10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE10" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH10" s="6" t="s">
         <v>28</v>
@@ -2095,16 +2089,16 @@
         <v>34</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO10" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ10" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.35">
@@ -2112,46 +2106,46 @@
         <v>37</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>10</v>
@@ -2163,49 +2157,49 @@
         <v>12</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="V11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X11" s="1" t="s">
+      <c r="AB11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AD11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE11" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH11" s="6" t="s">
         <v>28</v>
@@ -2226,16 +2220,16 @@
         <v>34</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO11" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ11" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.35">
@@ -2243,19 +2237,19 @@
         <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>3</v>
@@ -2273,19 +2267,19 @@
         <v>5</v>
       </c>
       <c r="L12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>10</v>
@@ -2294,49 +2288,49 @@
         <v>12</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="V12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X12" s="1" t="s">
+      <c r="AB12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AD12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH12" s="6" t="s">
         <v>29</v>
@@ -2357,16 +2351,16 @@
         <v>34</v>
       </c>
       <c r="AN12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ12" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ12" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:43" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -2380,13 +2374,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>3</v>
@@ -2410,10 +2404,10 @@
         <v>13</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>10</v>
@@ -2437,34 +2431,34 @@
         <v>21</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y13" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG13" s="6" t="s">
         <v>28</v>
@@ -2485,10 +2479,10 @@
         <v>31</v>
       </c>
       <c r="AM13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AN13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AO13" s="9" t="s">
         <v>35</v>
@@ -2497,7 +2491,7 @@
         <v>35</v>
       </c>
       <c r="AQ13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.35">
@@ -2511,13 +2505,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>3</v>
@@ -2541,10 +2535,10 @@
         <v>13</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>10</v>
@@ -2565,31 +2559,31 @@
         <v>15</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE14" s="6" t="s">
         <v>25</v>
@@ -2616,7 +2610,7 @@
         <v>31</v>
       </c>
       <c r="AM14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AN14" s="6" t="s">
         <v>34</v>
@@ -2625,10 +2619,10 @@
         <v>35</v>
       </c>
       <c r="AP14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AQ14" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.35">
@@ -2642,13 +2636,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>3</v>
@@ -2657,10 +2651,10 @@
         <v>3</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>5</v>
@@ -2669,13 +2663,13 @@
         <v>7</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>10</v>
@@ -2693,43 +2687,43 @@
         <v>19</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Z15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AB15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH15" s="6" t="s">
         <v>31</v>
@@ -2750,7 +2744,7 @@
         <v>34</v>
       </c>
       <c r="AN15" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AO15" s="9" t="s">
         <v>35</v>
@@ -2759,7 +2753,7 @@
         <v>35</v>
       </c>
       <c r="AQ15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.35">
@@ -2773,13 +2767,13 @@
         <v>0</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>3</v>
@@ -2803,10 +2797,10 @@
         <v>13</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>10</v>
@@ -2827,37 +2821,37 @@
         <v>21</v>
       </c>
       <c r="V16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF16" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG16" s="6" t="s">
         <v>28</v>
@@ -2904,13 +2898,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>3</v>
@@ -2934,10 +2928,10 @@
         <v>13</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>10</v>
@@ -2964,31 +2958,31 @@
         <v>16</v>
       </c>
       <c r="X17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y17" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="AD17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF17" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG17" s="6" t="s">
         <v>28</v>
@@ -3026,7 +3020,7 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>34</v>
@@ -3035,13 +3029,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>3</v>
@@ -3068,7 +3062,7 @@
         <v>9</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>10</v>
@@ -3083,43 +3077,43 @@
         <v>13</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF18" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG18" s="6" t="s">
         <v>28</v>
@@ -3166,13 +3160,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>3</v>
@@ -3196,10 +3190,10 @@
         <v>13</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>10</v>
@@ -3217,40 +3211,40 @@
         <v>18</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Y19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z19" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE19" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF19" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG19" s="6" t="s">
         <v>28</v>
@@ -3274,7 +3268,7 @@
         <v>34</v>
       </c>
       <c r="AN19" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AO19" s="9" t="s">
         <v>35</v>
@@ -3283,7 +3277,7 @@
         <v>35</v>
       </c>
       <c r="AQ19" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.35">
@@ -3291,19 +3285,19 @@
         <v>52</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>3</v>
@@ -3327,10 +3321,10 @@
         <v>13</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>10</v>
@@ -3345,43 +3339,43 @@
         <v>13</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF20" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG20" s="6" t="s">
         <v>28</v>
@@ -3405,16 +3399,16 @@
         <v>34</v>
       </c>
       <c r="AN20" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO20" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ20" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.35">
@@ -3428,13 +3422,13 @@
         <v>0</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>3</v>
@@ -3455,13 +3449,13 @@
         <v>7</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>10</v>
@@ -3476,46 +3470,46 @@
         <v>13</v>
       </c>
       <c r="T21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="V21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X21" s="1" t="s">
+      <c r="AB21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z21" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AD21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB21" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD21" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG21" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AH21" s="6" t="s">
         <v>28</v>
@@ -3533,19 +3527,19 @@
         <v>31</v>
       </c>
       <c r="AM21" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AN21" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AO21" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AP21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ21" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ21" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.35">
@@ -3559,13 +3553,13 @@
         <v>0</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>3</v>
@@ -3586,13 +3580,13 @@
         <v>7</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>10</v>
@@ -3607,49 +3601,49 @@
         <v>13</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W22" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y22" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG22" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI22" s="6" t="s">
         <v>29</v>
@@ -3673,10 +3667,10 @@
         <v>35</v>
       </c>
       <c r="AP22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AQ22" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.35">
@@ -3690,13 +3684,13 @@
         <v>0</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>3</v>
@@ -3720,10 +3714,10 @@
         <v>13</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P23" s="6" t="s">
         <v>10</v>
@@ -3738,43 +3732,43 @@
         <v>13</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Z23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG23" s="6" t="s">
         <v>28</v>
@@ -3795,10 +3789,10 @@
         <v>31</v>
       </c>
       <c r="AM23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AN23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AO23" s="9" t="s">
         <v>35</v>
@@ -3815,19 +3809,19 @@
         <v>56</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>3</v>
@@ -3848,13 +3842,13 @@
         <v>7</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>10</v>
@@ -3869,43 +3863,43 @@
         <v>13</v>
       </c>
       <c r="T24" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U24" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y24" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG24" s="6" t="s">
         <v>28</v>
@@ -3929,16 +3923,16 @@
         <v>34</v>
       </c>
       <c r="AN24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AO24" s="9" t="s">
         <v>35</v>
       </c>
       <c r="AP24" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AQ24" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.35">
@@ -3946,19 +3940,19 @@
         <v>57</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>3</v>
@@ -3967,25 +3961,25 @@
         <v>3</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>10</v>
@@ -3997,49 +3991,49 @@
         <v>12</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U25" s="1" t="s">
+      <c r="V25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA25" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA25" s="1" t="s">
+      <c r="AB25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE25" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AB25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE25" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="AF25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH25" s="6" t="s">
         <v>28</v>
@@ -4060,16 +4054,16 @@
         <v>34</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AO25" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AP25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ25" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AQ25" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.35">
@@ -4077,19 +4071,19 @@
         <v>58</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>3</v>
@@ -4098,25 +4092,25 @@
         <v>3</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>10</v>
@@ -4128,49 +4122,49 @@
         <v>12</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T26" s="6" t="s">
         <v>23</v>
       </c>
       <c r="U26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Z26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG26" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AH26" s="6" t="s">
         <v>28</v>
@@ -4200,7 +4194,7 @@
         <v>35</v>
       </c>
       <c r="AQ26" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.35">
@@ -4214,13 +4208,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>3</v>
@@ -4244,10 +4238,10 @@
         <v>13</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>10</v>
@@ -4262,10 +4256,10 @@
         <v>13</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="U27" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V27" s="6" t="s">
         <v>17</v>
@@ -4280,25 +4274,25 @@
         <v>18</v>
       </c>
       <c r="Z27" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA27" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AB27" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC27" s="6" t="s">
         <v>22</v>
       </c>
       <c r="AD27" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE27" s="6" t="s">
         <v>26</v>
       </c>
       <c r="AF27" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG27" s="6" t="s">
         <v>28</v>
@@ -4345,13 +4339,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>3</v>
@@ -4375,10 +4369,10 @@
         <v>13</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P28" s="6" t="s">
         <v>10</v>
@@ -4393,43 +4387,43 @@
         <v>13</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Z28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG28" s="6" t="s">
         <v>28</v>
@@ -4459,10 +4453,10 @@
         <v>35</v>
       </c>
       <c r="AP28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AQ28" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.35">
@@ -4476,13 +4470,13 @@
         <v>0</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>3</v>
@@ -4506,10 +4500,10 @@
         <v>13</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P29" s="6" t="s">
         <v>10</v>
@@ -4524,43 +4518,43 @@
         <v>13</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y29" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF29" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG29" s="6" t="s">
         <v>28</v>
@@ -4601,22 +4595,22 @@
         <v>62</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>3</v>
@@ -4637,10 +4631,10 @@
         <v>13</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P30" s="6" t="s">
         <v>11</v>
@@ -4655,43 +4649,43 @@
         <v>13</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Z30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG30" s="6" t="s">
         <v>28</v>
@@ -4712,7 +4706,7 @@
         <v>31</v>
       </c>
       <c r="AM30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AN30" s="6" t="s">
         <v>34</v>
@@ -4721,15 +4715,15 @@
         <v>35</v>
       </c>
       <c r="AP30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AQ30" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>34</v>
@@ -4738,13 +4732,13 @@
         <v>0</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>3</v>
@@ -4768,10 +4762,10 @@
         <v>13</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P31" s="6" t="s">
         <v>10</v>
@@ -4786,43 +4780,43 @@
         <v>13</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y31" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF31" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG31" s="6" t="s">
         <v>28</v>
@@ -4869,13 +4863,13 @@
         <v>0</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>3</v>
@@ -4899,10 +4893,10 @@
         <v>13</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P32" s="6" t="s">
         <v>10</v>
@@ -4917,43 +4911,43 @@
         <v>13</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W32" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y32" s="6" t="s">
         <v>18</v>
       </c>
       <c r="Z32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF32" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AG32" s="6" t="s">
         <v>28</v>
@@ -4991,526 +4985,264 @@
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>13</v>
+        <v>64</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R33" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="S33" s="6" t="s">
-        <v>13</v>
+        <v>66</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W33" s="6" t="s">
-        <v>16</v>
+        <v>66</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="X33" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y33" s="6" t="s">
-        <v>18</v>
+        <v>66</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="Z33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AB33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AC33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AD33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AE33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AF33" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK33" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL33" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO33" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ33" s="6" t="s">
-        <v>23</v>
+        <v>66</v>
+      </c>
+      <c r="AG33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ33" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="O34" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="P34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="S34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="T34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="U34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="V34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="X34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y34" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG34" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH34" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM34" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN34" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO34" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP34" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ34" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="L35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="N35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="O35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="P35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="R35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="S35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="T35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="U35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="V35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="X35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ35" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="W36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AN36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ36" s="1" t="s">
-        <v>78</v>
+      <c r="C34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ34" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>